<commit_message>
add encrypt python pyx to pyd
</commit_message>
<xml_diff>
--- a/upload/Siuuu.xlsx
+++ b/upload/Siuuu.xlsx
@@ -430,7 +430,7 @@
   <cols>
     <col width="19" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
@@ -468,26 +468,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>P-20250927_105039</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>E:\storage\901.mp4</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>sda</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
   </sheetData>
   <autoFilter ref="A1:F2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixing save problem and mapping folder
</commit_message>
<xml_diff>
--- a/upload/Siuuu.xlsx
+++ b/upload/Siuuu.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -429,52 +429,58 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="2" customWidth="1" min="7" max="7"/>
+    <col width="34" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>channel</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>directory</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>publish_date</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>publish_time</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>move_folder</t>
+        </is>
+      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>monetization</t>
         </is>
       </c>
     </row>
+    <row r="2"/>
   </sheetData>
   <autoFilter ref="A1:H2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>